<commit_message>
added data correction notebook for change provenance, build spider2 query methods
</commit_message>
<xml_diff>
--- a/subsetting_results/subsetting-chess-snails-Native-gpt4o.xlsx
+++ b/subsetting_results/subsetting-chess-snails-Native-gpt4o.xlsx
@@ -559,7 +559,7 @@
         <v>29.22348719998263</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1936469</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -639,7 +639,7 @@
         <v>38.60608329996467</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1928767</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -719,7 +719,7 @@
         <v>24.97183609998319</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1925965</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -799,7 +799,7 @@
         <v>28.27109579998069</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1927747</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -879,7 +879,7 @@
         <v>28.23576459998731</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1928765</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -959,7 +959,7 @@
         <v>30.16795200004708</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1929754</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -1039,7 +1039,7 @@
         <v>34.02543010003865</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>967500</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>30.99802639998961</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>968626</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -1199,7 +1199,7 @@
         <v>27.41357269999571</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>965122</v>
       </c>
       <c r="F10" t="n">
         <v>0.8</v>
@@ -1279,7 +1279,7 @@
         <v>32.89658010005951</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>968871</v>
       </c>
       <c r="F11" t="n">
         <v>0.625</v>
@@ -1359,7 +1359,7 @@
         <v>48.87115670007188</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>969122</v>
       </c>
       <c r="F12" t="n">
         <v>0.75</v>
@@ -1439,7 +1439,7 @@
         <v>32.80081709998194</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>964082</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -1519,7 +1519,7 @@
         <v>39.96331639995333</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>965587</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -1599,7 +1599,7 @@
         <v>34.60976259992458</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>965633</v>
       </c>
       <c r="F15" t="n">
         <v>0.75</v>
@@ -1679,7 +1679,7 @@
         <v>32.03661119996104</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>963680</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -1759,7 +1759,7 @@
         <v>33.57681580004282</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>963308</v>
       </c>
       <c r="F17" t="n">
         <v>0.4444444444444444</v>
@@ -1839,7 +1839,7 @@
         <v>30.97745740006212</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>966704</v>
       </c>
       <c r="F18" t="n">
         <v>0.6153846153846154</v>
@@ -1919,7 +1919,7 @@
         <v>36.41988499998115</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>967224</v>
       </c>
       <c r="F19" t="n">
         <v>0.6666666666666666</v>
@@ -1999,7 +1999,7 @@
         <v>28.54444480000529</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>964984</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -2079,7 +2079,7 @@
         <v>34.74986320000608</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>971146</v>
       </c>
       <c r="F21" t="n">
         <v>0.3333333333333333</v>
@@ -2159,7 +2159,7 @@
         <v>45.9211181999417</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>964162</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -2239,7 +2239,7 @@
         <v>36.81987140001729</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>964674</v>
       </c>
       <c r="F23" t="n">
         <v>0.75</v>
@@ -2319,7 +2319,7 @@
         <v>30.98569469992071</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>967405</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
@@ -2399,7 +2399,7 @@
         <v>40.65613819996361</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>967774</v>
       </c>
       <c r="F25" t="n">
         <v>0.7142857142857143</v>
@@ -2479,7 +2479,7 @@
         <v>31.23192469996866</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>969126</v>
       </c>
       <c r="F26" t="n">
         <v>0.5454545454545454</v>
@@ -2559,7 +2559,7 @@
         <v>60.32627610000782</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>967579</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -2639,7 +2639,7 @@
         <v>35.87470389995724</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>968158</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -2719,7 +2719,7 @@
         <v>42.23448950005695</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>973827</v>
       </c>
       <c r="F29" t="n">
         <v>0.7692307692307693</v>
@@ -2799,7 +2799,7 @@
         <v>35.50456050003413</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>966909</v>
       </c>
       <c r="F30" t="n">
         <v>0.2222222222222222</v>
@@ -2879,7 +2879,7 @@
         <v>32.02376039989758</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>968606</v>
       </c>
       <c r="F31" t="n">
         <v>1</v>
@@ -2959,7 +2959,7 @@
         <v>30.62022450007498</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>968261</v>
       </c>
       <c r="F32" t="n">
         <v>0.5555555555555556</v>
@@ -3039,7 +3039,7 @@
         <v>32.1909068999812</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>965897</v>
       </c>
       <c r="F33" t="n">
         <v>1</v>
@@ -3119,7 +3119,7 @@
         <v>31.57516129990108</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>963839</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -3199,7 +3199,7 @@
         <v>29.07267319993116</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>964787</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -3279,7 +3279,7 @@
         <v>29.61606210004538</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>963163</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -3359,7 +3359,7 @@
         <v>28.38798589992803</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>966189</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -3439,7 +3439,7 @@
         <v>33.21621350001078</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>965374</v>
       </c>
       <c r="F38" t="n">
         <v>1</v>
@@ -3519,7 +3519,7 @@
         <v>28.47281810001004</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>965320</v>
       </c>
       <c r="F39" t="n">
         <v>0.6</v>
@@ -3599,7 +3599,7 @@
         <v>28.93070780008566</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>968390</v>
       </c>
       <c r="F40" t="n">
         <v>1</v>
@@ -3679,7 +3679,7 @@
         <v>34.63407310005277</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>969632</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -3759,7 +3759,7 @@
         <v>31.3888001999585</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>759743</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -3839,7 +3839,7 @@
         <v>34.77060090005398</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>758569</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -3919,7 +3919,7 @@
         <v>38.42395800002851</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>760328</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -3999,7 +3999,7 @@
         <v>27.96656869992148</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>756023</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
@@ -4079,7 +4079,7 @@
         <v>28.97447160002775</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>756971</v>
       </c>
       <c r="F46" t="n">
         <v>1</v>
@@ -4159,7 +4159,7 @@
         <v>27.43602179992013</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>757646</v>
       </c>
       <c r="F47" t="n">
         <v>1</v>
@@ -4239,7 +4239,7 @@
         <v>46.291490899981</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>761042</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -4319,7 +4319,7 @@
         <v>35.66169109998737</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>762120</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
@@ -4399,7 +4399,7 @@
         <v>37.24682300002314</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>760720</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -4479,7 +4479,7 @@
         <v>31.20602569996845</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>757789</v>
       </c>
       <c r="F51" t="n">
         <v>1</v>
@@ -4559,7 +4559,7 @@
         <v>31.05121000006329</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>757939</v>
       </c>
       <c r="F52" t="n">
         <v>1</v>
@@ -4639,7 +4639,7 @@
         <v>30.81941669993103</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>759777</v>
       </c>
       <c r="F53" t="n">
         <v>1</v>
@@ -4719,7 +4719,7 @@
         <v>35.98205780005082</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>759012</v>
       </c>
       <c r="F54" t="n">
         <v>1</v>
@@ -4799,7 +4799,7 @@
         <v>33.53649870003574</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>759130</v>
       </c>
       <c r="F55" t="n">
         <v>1</v>
@@ -4879,7 +4879,7 @@
         <v>29.02285930002108</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>756322</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
@@ -4959,7 +4959,7 @@
         <v>27.17433199996594</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>756139</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
@@ -5039,7 +5039,7 @@
         <v>28.19210139999632</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>758505</v>
       </c>
       <c r="F58" t="n">
         <v>0.8333333333333334</v>
@@ -5119,7 +5119,7 @@
         <v>49.66828000009991</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>758028</v>
       </c>
       <c r="F59" t="n">
         <v>0.5</v>
@@ -5199,7 +5199,7 @@
         <v>29.79483799997251</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>758821</v>
       </c>
       <c r="F60" t="n">
         <v>1</v>
@@ -5279,7 +5279,7 @@
         <v>28.73596489999909</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>759587</v>
       </c>
       <c r="F61" t="n">
         <v>0.75</v>
@@ -5359,7 +5359,7 @@
         <v>34.66122940008063</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>757899</v>
       </c>
       <c r="F62" t="n">
         <v>1</v>
@@ -5439,7 +5439,7 @@
         <v>29.14542119996622</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>759294</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
@@ -5519,7 +5519,7 @@
         <v>51.66315270005725</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>756523</v>
       </c>
       <c r="F64" t="n">
         <v>0.8888888888888888</v>
@@ -5599,7 +5599,7 @@
         <v>42.96088280004915</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>759760</v>
       </c>
       <c r="F65" t="n">
         <v>1</v>
@@ -5679,7 +5679,7 @@
         <v>38.51725709997118</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>760804</v>
       </c>
       <c r="F66" t="n">
         <v>1</v>
@@ -5759,7 +5759,7 @@
         <v>27.92232799995691</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>757589</v>
       </c>
       <c r="F67" t="n">
         <v>1</v>
@@ -5839,7 +5839,7 @@
         <v>32.76642179989722</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>757292</v>
       </c>
       <c r="F68" t="n">
         <v>1</v>
@@ -5919,7 +5919,7 @@
         <v>36.49154050007928</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>756471</v>
       </c>
       <c r="F69" t="n">
         <v>1</v>
@@ -5999,7 +5999,7 @@
         <v>33.23769300000276</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>762139</v>
       </c>
       <c r="F70" t="n">
         <v>0.7222222222222222</v>
@@ -6079,7 +6079,7 @@
         <v>34.48700289998669</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>758419</v>
       </c>
       <c r="F71" t="n">
         <v>0.6</v>
@@ -6159,7 +6159,7 @@
         <v>30.552786400076</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>757453</v>
       </c>
       <c r="F72" t="n">
         <v>1</v>
@@ -6239,7 +6239,7 @@
         <v>30.32311280001886</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>758248</v>
       </c>
       <c r="F73" t="n">
         <v>0.8</v>
@@ -6319,7 +6319,7 @@
         <v>39.23357549996581</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>762655</v>
       </c>
       <c r="F74" t="n">
         <v>1</v>
@@ -6399,7 +6399,7 @@
         <v>30.73197429999709</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>758038</v>
       </c>
       <c r="F75" t="n">
         <v>1</v>
@@ -6479,7 +6479,7 @@
         <v>23.8772904999787</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>757466</v>
       </c>
       <c r="F76" t="n">
         <v>1</v>
@@ -6559,7 +6559,7 @@
         <v>32.23456740006804</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>758188</v>
       </c>
       <c r="F77" t="n">
         <v>0.8</v>
@@ -6639,7 +6639,7 @@
         <v>30.81656319997273</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>757417</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
@@ -6719,7 +6719,7 @@
         <v>34.82757399999537</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>760632</v>
       </c>
       <c r="F79" t="n">
         <v>1</v>
@@ -6799,7 +6799,7 @@
         <v>34.12378969998099</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>758080</v>
       </c>
       <c r="F80" t="n">
         <v>1</v>
@@ -6879,7 +6879,7 @@
         <v>40.19565439992584</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>758178</v>
       </c>
       <c r="F81" t="n">
         <v>1</v>
@@ -6959,7 +6959,7 @@
         <v>32.78104560007341</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>281283</v>
       </c>
       <c r="F82" t="n">
         <v>0.75</v>
@@ -7039,7 +7039,7 @@
         <v>28.81734969990794</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>281153</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
@@ -7119,7 +7119,7 @@
         <v>31.26216059993021</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>282535</v>
       </c>
       <c r="F84" t="n">
         <v>0.8333333333333334</v>
@@ -7199,7 +7199,7 @@
         <v>29.84562380006537</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>281769</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
@@ -7279,7 +7279,7 @@
         <v>32.31241320003755</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>282564</v>
       </c>
       <c r="F86" t="n">
         <v>1</v>
@@ -7359,7 +7359,7 @@
         <v>27.55329380009789</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>281637</v>
       </c>
       <c r="F87" t="n">
         <v>1</v>
@@ -7439,7 +7439,7 @@
         <v>28.87458569998853</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>281468</v>
       </c>
       <c r="F88" t="n">
         <v>1</v>
@@ -7519,7 +7519,7 @@
         <v>24.52106800000183</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>281066</v>
       </c>
       <c r="F89" t="n">
         <v>0.6666666666666666</v>
@@ -7599,7 +7599,7 @@
         <v>30.6090591000393</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>281465</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
@@ -7679,7 +7679,7 @@
         <v>25.35204419994261</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>281508</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
@@ -7759,7 +7759,7 @@
         <v>25.30250630003866</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>281604</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -7839,7 +7839,7 @@
         <v>28.85783420002554</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>281729</v>
       </c>
       <c r="F93" t="n">
         <v>1</v>
@@ -7919,7 +7919,7 @@
         <v>27.79118790000211</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>281152</v>
       </c>
       <c r="F94" t="n">
         <v>1</v>
@@ -7999,7 +7999,7 @@
         <v>32.35344750003424</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>283718</v>
       </c>
       <c r="F95" t="n">
         <v>0.8</v>
@@ -8079,7 +8079,7 @@
         <v>34.44675889995415</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>284029</v>
       </c>
       <c r="F96" t="n">
         <v>0.9090909090909091</v>
@@ -8159,7 +8159,7 @@
         <v>24.98881680006161</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>281189</v>
       </c>
       <c r="F97" t="n">
         <v>1</v>
@@ -8239,7 +8239,7 @@
         <v>30.84691930003464</v>
       </c>
       <c r="E98" t="n">
-        <v>0</v>
+        <v>281541</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
@@ -8319,7 +8319,7 @@
         <v>32.08616810000967</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>281883</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -8399,7 +8399,7 @@
         <v>32.78905420005322</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>282271</v>
       </c>
       <c r="F100" t="n">
         <v>0.5</v>
@@ -8479,7 +8479,7 @@
         <v>31.24506149999797</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>282775</v>
       </c>
       <c r="F101" t="n">
         <v>0.8</v>
@@ -8559,7 +8559,7 @@
         <v>35.51120690000243</v>
       </c>
       <c r="E102" t="n">
-        <v>0</v>
+        <v>282269</v>
       </c>
       <c r="F102" t="n">
         <v>0.4</v>
@@ -8639,7 +8639,7 @@
         <v>34.6843455999624</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>282334</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
@@ -8719,7 +8719,7 @@
         <v>27.0452990999911</v>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
+        <v>280947</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
@@ -8799,7 +8799,7 @@
         <v>26.51812499994412</v>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
+        <v>281834</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
@@ -8879,7 +8879,7 @@
         <v>30.1062584000174</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>281641</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
@@ -8959,7 +8959,7 @@
         <v>29.05175319989212</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>281630</v>
       </c>
       <c r="F107" t="n">
         <v>1</v>
@@ -9039,7 +9039,7 @@
         <v>30.01004339999054</v>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>281610</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
@@ -9119,7 +9119,7 @@
         <v>24.94651800009888</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>282080</v>
       </c>
       <c r="F109" t="n">
         <v>1</v>
@@ -9199,7 +9199,7 @@
         <v>28.3936732999282</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>281015</v>
       </c>
       <c r="F110" t="n">
         <v>0.4</v>
@@ -9279,7 +9279,7 @@
         <v>35.94503469998017</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>282886</v>
       </c>
       <c r="F111" t="n">
         <v>0.8888888888888888</v>
@@ -9359,7 +9359,7 @@
         <v>29.41305229999125</v>
       </c>
       <c r="E112" t="n">
-        <v>0</v>
+        <v>281494</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -9439,7 +9439,7 @@
         <v>29.23434939992148</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>281905</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>
@@ -9519,7 +9519,7 @@
         <v>28.87443530000746</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>282049</v>
       </c>
       <c r="F114" t="n">
         <v>1</v>
@@ -9599,7 +9599,7 @@
         <v>41.13244200008921</v>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>280939</v>
       </c>
       <c r="F115" t="n">
         <v>0.75</v>
@@ -9679,7 +9679,7 @@
         <v>28.54587519995403</v>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>281164</v>
       </c>
       <c r="F116" t="n">
         <v>1</v>
@@ -9759,7 +9759,7 @@
         <v>28.40277769998647</v>
       </c>
       <c r="E117" t="n">
-        <v>0</v>
+        <v>282020</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
@@ -9839,7 +9839,7 @@
         <v>32.04476219997741</v>
       </c>
       <c r="E118" t="n">
-        <v>0</v>
+        <v>282866</v>
       </c>
       <c r="F118" t="n">
         <v>1</v>
@@ -9919,7 +9919,7 @@
         <v>33.71765899995808</v>
       </c>
       <c r="E119" t="n">
-        <v>0</v>
+        <v>282263</v>
       </c>
       <c r="F119" t="n">
         <v>1</v>
@@ -9999,7 +9999,7 @@
         <v>28.47784900001716</v>
       </c>
       <c r="E120" t="n">
-        <v>0</v>
+        <v>282255</v>
       </c>
       <c r="F120" t="n">
         <v>0.8333333333333334</v>
@@ -10079,7 +10079,7 @@
         <v>21.53765509999357</v>
       </c>
       <c r="E121" t="n">
-        <v>0</v>
+        <v>280109</v>
       </c>
       <c r="F121" t="n">
         <v>1</v>
@@ -10159,7 +10159,7 @@
         <v>44.21463269996457</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>621362</v>
       </c>
       <c r="F122" t="n">
         <v>1</v>
@@ -10239,7 +10239,7 @@
         <v>41.97285279992502</v>
       </c>
       <c r="E123" t="n">
-        <v>0</v>
+        <v>621358</v>
       </c>
       <c r="F123" t="n">
         <v>0.5</v>
@@ -10319,7 +10319,7 @@
         <v>27.05364609998651</v>
       </c>
       <c r="E124" t="n">
-        <v>0</v>
+        <v>617427</v>
       </c>
       <c r="F124" t="n">
         <v>1</v>
@@ -10399,7 +10399,7 @@
         <v>32.5460036000004</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>618962</v>
       </c>
       <c r="F125" t="n">
         <v>1</v>
@@ -10479,7 +10479,7 @@
         <v>29.50744409998879</v>
       </c>
       <c r="E126" t="n">
-        <v>0</v>
+        <v>619986</v>
       </c>
       <c r="F126" t="n">
         <v>1</v>
@@ -10559,7 +10559,7 @@
         <v>31.27771779999603</v>
       </c>
       <c r="E127" t="n">
-        <v>0</v>
+        <v>623595</v>
       </c>
       <c r="F127" t="n">
         <v>1</v>
@@ -10639,7 +10639,7 @@
         <v>29.24286040000152</v>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
+        <v>619226</v>
       </c>
       <c r="F128" t="n">
         <v>1</v>
@@ -10719,7 +10719,7 @@
         <v>36.94877589994576</v>
       </c>
       <c r="E129" t="n">
-        <v>0</v>
+        <v>624054</v>
       </c>
       <c r="F129" t="n">
         <v>0.9230769230769231</v>
@@ -10799,7 +10799,7 @@
         <v>27.74605740001425</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>619484</v>
       </c>
       <c r="F130" t="n">
         <v>1</v>
@@ -10879,7 +10879,7 @@
         <v>34.95821409998462</v>
       </c>
       <c r="E131" t="n">
-        <v>0</v>
+        <v>620860</v>
       </c>
       <c r="F131" t="n">
         <v>1</v>
@@ -10959,7 +10959,7 @@
         <v>34.6343937999336</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>620949</v>
       </c>
       <c r="F132" t="n">
         <v>1</v>
@@ -11039,7 +11039,7 @@
         <v>35.82410920003895</v>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>620288</v>
       </c>
       <c r="F133" t="n">
         <v>1</v>
@@ -11119,7 +11119,7 @@
         <v>35.44444089999888</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>623436</v>
       </c>
       <c r="F134" t="n">
         <v>1</v>
@@ -11199,7 +11199,7 @@
         <v>30.37022479996085</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>622228</v>
       </c>
       <c r="F135" t="n">
         <v>1</v>
@@ -11279,7 +11279,7 @@
         <v>34.08653009997215</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>622476</v>
       </c>
       <c r="F136" t="n">
         <v>0.8571428571428571</v>
@@ -11359,7 +11359,7 @@
         <v>33.68359519995283</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>617780</v>
       </c>
       <c r="F137" t="n">
         <v>0.5</v>
@@ -11439,7 +11439,7 @@
         <v>34.40247490000911</v>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>617865</v>
       </c>
       <c r="F138" t="n">
         <v>1</v>
@@ -11519,7 +11519,7 @@
         <v>34.73922149999999</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
+        <v>619718</v>
       </c>
       <c r="F139" t="n">
         <v>0.75</v>
@@ -11599,7 +11599,7 @@
         <v>29.99157960002776</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>618571</v>
       </c>
       <c r="F140" t="n">
         <v>1</v>
@@ -11679,7 +11679,7 @@
         <v>34.41643390001263</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>619651</v>
       </c>
       <c r="F141" t="n">
         <v>0.375</v>
@@ -11759,7 +11759,7 @@
         <v>26.05974489997607</v>
       </c>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>619743</v>
       </c>
       <c r="F142" t="n">
         <v>1</v>
@@ -11839,7 +11839,7 @@
         <v>30.23407679994125</v>
       </c>
       <c r="E143" t="n">
-        <v>0</v>
+        <v>621826</v>
       </c>
       <c r="F143" t="n">
         <v>1</v>
@@ -11919,7 +11919,7 @@
         <v>32.63103320007212</v>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>620193</v>
       </c>
       <c r="F144" t="n">
         <v>0.6666666666666666</v>
@@ -11999,7 +11999,7 @@
         <v>41.43269539996982</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>637028</v>
       </c>
       <c r="F145" t="n">
         <v>1</v>
@@ -12079,7 +12079,7 @@
         <v>34.35643589997198</v>
       </c>
       <c r="E146" t="n">
-        <v>0</v>
+        <v>619889</v>
       </c>
       <c r="F146" t="n">
         <v>1</v>
@@ -12159,7 +12159,7 @@
         <v>27.41940779995639</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>619792</v>
       </c>
       <c r="F147" t="n">
         <v>0.8333333333333334</v>
@@ -12239,7 +12239,7 @@
         <v>36.1328182000434</v>
       </c>
       <c r="E148" t="n">
-        <v>0</v>
+        <v>624307</v>
       </c>
       <c r="F148" t="n">
         <v>1</v>
@@ -12319,7 +12319,7 @@
         <v>49.81280200008769</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>639179</v>
       </c>
       <c r="F149" t="n">
         <v>1</v>
@@ -12399,7 +12399,7 @@
         <v>36.99210979999043</v>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>623204</v>
       </c>
       <c r="F150" t="n">
         <v>1</v>
@@ -12479,7 +12479,7 @@
         <v>36.74877890001517</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>623552</v>
       </c>
       <c r="F151" t="n">
         <v>0.75</v>
@@ -12559,7 +12559,7 @@
         <v>26.47654389997479</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>618621</v>
       </c>
       <c r="F152" t="n">
         <v>1</v>
@@ -12639,7 +12639,7 @@
         <v>32.18438099999912</v>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>619374</v>
       </c>
       <c r="F153" t="n">
         <v>1</v>
@@ -12719,7 +12719,7 @@
         <v>33.19426380004734</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>621731</v>
       </c>
       <c r="F154" t="n">
         <v>0.8333333333333334</v>
@@ -12799,7 +12799,7 @@
         <v>39.05999610002618</v>
       </c>
       <c r="E155" t="n">
-        <v>0</v>
+        <v>620980</v>
       </c>
       <c r="F155" t="n">
         <v>1</v>
@@ -12879,7 +12879,7 @@
         <v>25.60179159999825</v>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>619152</v>
       </c>
       <c r="F156" t="n">
         <v>1</v>
@@ -12959,7 +12959,7 @@
         <v>29.60829220002051</v>
       </c>
       <c r="E157" t="n">
-        <v>0</v>
+        <v>620307</v>
       </c>
       <c r="F157" t="n">
         <v>0</v>
@@ -13039,7 +13039,7 @@
         <v>33.8573237999808</v>
       </c>
       <c r="E158" t="n">
-        <v>0</v>
+        <v>624526</v>
       </c>
       <c r="F158" t="n">
         <v>1</v>
@@ -13119,7 +13119,7 @@
         <v>34.71701719996054</v>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>619081</v>
       </c>
       <c r="F159" t="n">
         <v>1</v>
@@ -13199,7 +13199,7 @@
         <v>41.01587660005316</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>624515</v>
       </c>
       <c r="F160" t="n">
         <v>1</v>
@@ -13279,7 +13279,7 @@
         <v>35.51397219998762</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>623116</v>
       </c>
       <c r="F161" t="n">
         <v>0.9</v>
@@ -13359,7 +13359,7 @@
         <v>29.32023730000947</v>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>748448</v>
       </c>
       <c r="F162" t="n">
         <v>1</v>
@@ -13439,7 +13439,7 @@
         <v>28.0857682999922</v>
       </c>
       <c r="E163" t="n">
-        <v>0</v>
+        <v>750431</v>
       </c>
       <c r="F163" t="n">
         <v>0.6666666666666666</v>
@@ -13519,7 +13519,7 @@
         <v>32.52762599999551</v>
       </c>
       <c r="E164" t="n">
-        <v>0</v>
+        <v>748522</v>
       </c>
       <c r="F164" t="n">
         <v>1</v>
@@ -13599,7 +13599,7 @@
         <v>31.21007049991749</v>
       </c>
       <c r="E165" t="n">
-        <v>0</v>
+        <v>750266</v>
       </c>
       <c r="F165" t="n">
         <v>1</v>
@@ -13679,7 +13679,7 @@
         <v>29.02831510000397</v>
       </c>
       <c r="E166" t="n">
-        <v>0</v>
+        <v>754102</v>
       </c>
       <c r="F166" t="n">
         <v>0.75</v>
@@ -13759,7 +13759,7 @@
         <v>109.6751088000601</v>
       </c>
       <c r="E167" t="n">
-        <v>0</v>
+        <v>751719</v>
       </c>
       <c r="F167" t="n">
         <v>0.6666666666666666</v>
@@ -13839,7 +13839,7 @@
         <v>36.74155989999417</v>
       </c>
       <c r="E168" t="n">
-        <v>0</v>
+        <v>752075</v>
       </c>
       <c r="F168" t="n">
         <v>1</v>
@@ -13919,7 +13919,7 @@
         <v>32.19297610002104</v>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>748629</v>
       </c>
       <c r="F169" t="n">
         <v>1</v>
@@ -13999,7 +13999,7 @@
         <v>32.0848303999519</v>
       </c>
       <c r="E170" t="n">
-        <v>0</v>
+        <v>749877</v>
       </c>
       <c r="F170" t="n">
         <v>0.6</v>
@@ -14079,7 +14079,7 @@
         <v>46.71434730000328</v>
       </c>
       <c r="E171" t="n">
-        <v>0</v>
+        <v>751051</v>
       </c>
       <c r="F171" t="n">
         <v>0.8</v>
@@ -14159,7 +14159,7 @@
         <v>29.49353380000684</v>
       </c>
       <c r="E172" t="n">
-        <v>0</v>
+        <v>752066</v>
       </c>
       <c r="F172" t="n">
         <v>1</v>
@@ -14239,7 +14239,7 @@
         <v>35.62966590002179</v>
       </c>
       <c r="E173" t="n">
-        <v>0</v>
+        <v>751208</v>
       </c>
       <c r="F173" t="n">
         <v>1</v>
@@ -14319,7 +14319,7 @@
         <v>39.74109950009733</v>
       </c>
       <c r="E174" t="n">
-        <v>0</v>
+        <v>750060</v>
       </c>
       <c r="F174" t="n">
         <v>1</v>
@@ -14399,7 +14399,7 @@
         <v>53.46220149996225</v>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>775506</v>
       </c>
       <c r="F175" t="n">
         <v>0.8</v>
@@ -14479,7 +14479,7 @@
         <v>28.17838089994621</v>
       </c>
       <c r="E176" t="n">
-        <v>0</v>
+        <v>749484</v>
       </c>
       <c r="F176" t="n">
         <v>0.8</v>
@@ -14559,7 +14559,7 @@
         <v>30.02249910007231</v>
       </c>
       <c r="E177" t="n">
-        <v>0</v>
+        <v>752340</v>
       </c>
       <c r="F177" t="n">
         <v>1</v>
@@ -14639,7 +14639,7 @@
         <v>34.94034989993088</v>
       </c>
       <c r="E178" t="n">
-        <v>0</v>
+        <v>753723</v>
       </c>
       <c r="F178" t="n">
         <v>0.9</v>
@@ -14719,7 +14719,7 @@
         <v>27.96893400000408</v>
       </c>
       <c r="E179" t="n">
-        <v>0</v>
+        <v>751049</v>
       </c>
       <c r="F179" t="n">
         <v>1</v>
@@ -14799,7 +14799,7 @@
         <v>30.90575520007405</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>749661</v>
       </c>
       <c r="F180" t="n">
         <v>1</v>
@@ -14879,7 +14879,7 @@
         <v>29.81774760002736</v>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>747741</v>
       </c>
       <c r="F181" t="n">
         <v>1</v>
@@ -14959,7 +14959,7 @@
         <v>35.1919721000595</v>
       </c>
       <c r="E182" t="n">
-        <v>0</v>
+        <v>752182</v>
       </c>
       <c r="F182" t="n">
         <v>0.8571428571428571</v>
@@ -15039,7 +15039,7 @@
         <v>37.1852486000862</v>
       </c>
       <c r="E183" t="n">
-        <v>0</v>
+        <v>751728</v>
       </c>
       <c r="F183" t="n">
         <v>1</v>
@@ -15119,7 +15119,7 @@
         <v>29.33707759995013</v>
       </c>
       <c r="E184" t="n">
-        <v>0</v>
+        <v>753043</v>
       </c>
       <c r="F184" t="n">
         <v>1</v>
@@ -15199,7 +15199,7 @@
         <v>30.9687297999626</v>
       </c>
       <c r="E185" t="n">
-        <v>0</v>
+        <v>754266</v>
       </c>
       <c r="F185" t="n">
         <v>1</v>
@@ -15279,7 +15279,7 @@
         <v>26.17172730003949</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>749467</v>
       </c>
       <c r="F186" t="n">
         <v>1</v>
@@ -15359,7 +15359,7 @@
         <v>30.05938270001207</v>
       </c>
       <c r="E187" t="n">
-        <v>0</v>
+        <v>750852</v>
       </c>
       <c r="F187" t="n">
         <v>1</v>
@@ -15439,7 +15439,7 @@
         <v>36.51998230000027</v>
       </c>
       <c r="E188" t="n">
-        <v>0</v>
+        <v>752235</v>
       </c>
       <c r="F188" t="n">
         <v>0.9</v>
@@ -15519,7 +15519,7 @@
         <v>25.5819587999722</v>
       </c>
       <c r="E189" t="n">
-        <v>0</v>
+        <v>748706</v>
       </c>
       <c r="F189" t="n">
         <v>1</v>
@@ -15599,7 +15599,7 @@
         <v>35.62942020001356</v>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>751733</v>
       </c>
       <c r="F190" t="n">
         <v>1</v>
@@ -15679,7 +15679,7 @@
         <v>25.74217010010034</v>
       </c>
       <c r="E191" t="n">
-        <v>0</v>
+        <v>748178</v>
       </c>
       <c r="F191" t="n">
         <v>1</v>
@@ -15759,7 +15759,7 @@
         <v>32.92918360000476</v>
       </c>
       <c r="E192" t="n">
-        <v>0</v>
+        <v>751477</v>
       </c>
       <c r="F192" t="n">
         <v>0.8333333333333334</v>
@@ -15839,7 +15839,7 @@
         <v>33.48064820002764</v>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>752002</v>
       </c>
       <c r="F193" t="n">
         <v>0.3333333333333333</v>
@@ -15919,7 +15919,7 @@
         <v>29.01467349997256</v>
       </c>
       <c r="E194" t="n">
-        <v>0</v>
+        <v>750791</v>
       </c>
       <c r="F194" t="n">
         <v>1</v>
@@ -15999,7 +15999,7 @@
         <v>30.31028249999508</v>
       </c>
       <c r="E195" t="n">
-        <v>0</v>
+        <v>751618</v>
       </c>
       <c r="F195" t="n">
         <v>1</v>
@@ -16079,7 +16079,7 @@
         <v>29.53252949996386</v>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>748227</v>
       </c>
       <c r="F196" t="n">
         <v>0.8333333333333334</v>
@@ -16159,7 +16159,7 @@
         <v>30.36695960001089</v>
       </c>
       <c r="E197" t="n">
-        <v>0</v>
+        <v>751471</v>
       </c>
       <c r="F197" t="n">
         <v>1</v>
@@ -16239,7 +16239,7 @@
         <v>37.2886311999755</v>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>752004</v>
       </c>
       <c r="F198" t="n">
         <v>1</v>
@@ -16319,7 +16319,7 @@
         <v>34.81236169999465</v>
       </c>
       <c r="E199" t="n">
-        <v>0</v>
+        <v>752036</v>
       </c>
       <c r="F199" t="n">
         <v>0.8333333333333334</v>
@@ -16399,7 +16399,7 @@
         <v>28.8719174999278</v>
       </c>
       <c r="E200" t="n">
-        <v>0</v>
+        <v>751253</v>
       </c>
       <c r="F200" t="n">
         <v>1</v>
@@ -16479,7 +16479,7 @@
         <v>26.34132230002433</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>749403</v>
       </c>
       <c r="F201" t="n">
         <v>1</v>
@@ -16559,7 +16559,7 @@
         <v>64.01033549988642</v>
       </c>
       <c r="E202" t="n">
-        <v>0</v>
+        <v>4555021</v>
       </c>
       <c r="F202" t="n">
         <v>0.5</v>
@@ -16639,7 +16639,7 @@
         <v>69.06357909995131</v>
       </c>
       <c r="E203" t="n">
-        <v>0</v>
+        <v>4555030</v>
       </c>
       <c r="F203" t="n">
         <v>0.5</v>
@@ -16719,7 +16719,7 @@
         <v>72.4510314000072</v>
       </c>
       <c r="E204" t="n">
-        <v>0</v>
+        <v>4554722</v>
       </c>
       <c r="F204" t="n">
         <v>1</v>
@@ -16799,7 +16799,7 @@
         <v>50.09784070006572</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>4562249</v>
       </c>
       <c r="F205" t="n">
         <v>1</v>
@@ -16879,7 +16879,7 @@
         <v>47.17214830010198</v>
       </c>
       <c r="E206" t="n">
-        <v>0</v>
+        <v>4557988</v>
       </c>
       <c r="F206" t="n">
         <v>0.5</v>
@@ -16959,7 +16959,7 @@
         <v>64.06786979991011</v>
       </c>
       <c r="E207" t="n">
-        <v>0</v>
+        <v>4570852</v>
       </c>
       <c r="F207" t="n">
         <v>1</v>
@@ -17039,7 +17039,7 @@
         <v>52.10852670005988</v>
       </c>
       <c r="E208" t="n">
-        <v>0</v>
+        <v>4565999</v>
       </c>
       <c r="F208" t="n">
         <v>1</v>
@@ -17119,7 +17119,7 @@
         <v>58.68880370003171</v>
       </c>
       <c r="E209" t="n">
-        <v>0</v>
+        <v>4571789</v>
       </c>
       <c r="F209" t="n">
         <v>1</v>
@@ -17199,7 +17199,7 @@
         <v>56.02790970006026</v>
       </c>
       <c r="E210" t="n">
-        <v>0</v>
+        <v>4587143</v>
       </c>
       <c r="F210" t="n">
         <v>1</v>
@@ -17279,7 +17279,7 @@
         <v>52.26329710008577</v>
       </c>
       <c r="E211" t="n">
-        <v>0</v>
+        <v>4584753</v>
       </c>
       <c r="F211" t="n">
         <v>0.2727272727272727</v>
@@ -17359,7 +17359,7 @@
         <v>45.96482669992838</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>4554772</v>
       </c>
       <c r="F212" t="n">
         <v>1</v>
@@ -17439,7 +17439,7 @@
         <v>50.76596470002551</v>
       </c>
       <c r="E213" t="n">
-        <v>0</v>
+        <v>4554346</v>
       </c>
       <c r="F213" t="n">
         <v>1</v>
@@ -17519,7 +17519,7 @@
         <v>56.02256020007189</v>
       </c>
       <c r="E214" t="n">
-        <v>0</v>
+        <v>4596312</v>
       </c>
       <c r="F214" t="n">
         <v>0.6666666666666666</v>
@@ -17599,7 +17599,7 @@
         <v>57.07815730001312</v>
       </c>
       <c r="E215" t="n">
-        <v>0</v>
+        <v>4566664</v>
       </c>
       <c r="F215" t="n">
         <v>1</v>
@@ -17679,7 +17679,7 @@
         <v>55.22959360003006</v>
       </c>
       <c r="E216" t="n">
-        <v>0</v>
+        <v>4611651</v>
       </c>
       <c r="F216" t="n">
         <v>0.3333333333333333</v>
@@ -17759,7 +17759,7 @@
         <v>58.41414469992742</v>
       </c>
       <c r="E217" t="n">
-        <v>0</v>
+        <v>4597255</v>
       </c>
       <c r="F217" t="n">
         <v>1</v>
@@ -17839,7 +17839,7 @@
         <v>54.26534449995961</v>
       </c>
       <c r="E218" t="n">
-        <v>0</v>
+        <v>4586316</v>
       </c>
       <c r="F218" t="n">
         <v>0</v>
@@ -17919,7 +17919,7 @@
         <v>47.07598979992326</v>
       </c>
       <c r="E219" t="n">
-        <v>0</v>
+        <v>4559356</v>
       </c>
       <c r="F219" t="n">
         <v>0.75</v>
@@ -17999,7 +17999,7 @@
         <v>63.87005150003824</v>
       </c>
       <c r="E220" t="n">
-        <v>0</v>
+        <v>4560217</v>
       </c>
       <c r="F220" t="n">
         <v>1</v>
@@ -18079,7 +18079,7 @@
         <v>103.6722589000128</v>
       </c>
       <c r="E221" t="n">
-        <v>0</v>
+        <v>4589728</v>
       </c>
       <c r="F221" t="n">
         <v>1</v>
@@ -18159,7 +18159,7 @@
         <v>73.05740839999635</v>
       </c>
       <c r="E222" t="n">
-        <v>0</v>
+        <v>4575057</v>
       </c>
       <c r="F222" t="n">
         <v>1</v>
@@ -18239,7 +18239,7 @@
         <v>102.0844969999744</v>
       </c>
       <c r="E223" t="n">
-        <v>0</v>
+        <v>4556255</v>
       </c>
       <c r="F223" t="n">
         <v>0</v>
@@ -18319,7 +18319,7 @@
         <v>82.09539439994842</v>
       </c>
       <c r="E224" t="n">
-        <v>0</v>
+        <v>4553473</v>
       </c>
       <c r="F224" t="n">
         <v>0.5</v>
@@ -18399,7 +18399,7 @@
         <v>58.17826039995998</v>
       </c>
       <c r="E225" t="n">
-        <v>0</v>
+        <v>4576627</v>
       </c>
       <c r="F225" t="n">
         <v>0</v>
@@ -18479,7 +18479,7 @@
         <v>63.35232279996853</v>
       </c>
       <c r="E226" t="n">
-        <v>0</v>
+        <v>4575462</v>
       </c>
       <c r="F226" t="n">
         <v>0.6666666666666666</v>
@@ -18559,7 +18559,7 @@
         <v>57.48802149994299</v>
       </c>
       <c r="E227" t="n">
-        <v>0</v>
+        <v>4577766</v>
       </c>
       <c r="F227" t="n">
         <v>0.3333333333333333</v>
@@ -18639,7 +18639,7 @@
         <v>52.3356088999426</v>
       </c>
       <c r="E228" t="n">
-        <v>0</v>
+        <v>4573024</v>
       </c>
       <c r="F228" t="n">
         <v>0.875</v>
@@ -18719,7 +18719,7 @@
         <v>68.29420789994765</v>
       </c>
       <c r="E229" t="n">
-        <v>0</v>
+        <v>4550015</v>
       </c>
       <c r="F229" t="n">
         <v>0.75</v>
@@ -18799,7 +18799,7 @@
         <v>138.4979895999422</v>
       </c>
       <c r="E230" t="n">
-        <v>0</v>
+        <v>4586506</v>
       </c>
       <c r="F230" t="n">
         <v>1</v>
@@ -18879,7 +18879,7 @@
         <v>60.7445510000689</v>
       </c>
       <c r="E231" t="n">
-        <v>0</v>
+        <v>4588726</v>
       </c>
       <c r="F231" t="n">
         <v>0</v>
@@ -18959,7 +18959,7 @@
         <v>62.93134110001847</v>
       </c>
       <c r="E232" t="n">
-        <v>0</v>
+        <v>4593921</v>
       </c>
       <c r="F232" t="n">
         <v>0</v>
@@ -19039,7 +19039,7 @@
         <v>61.11792210000567</v>
       </c>
       <c r="E233" t="n">
-        <v>0</v>
+        <v>4595051</v>
       </c>
       <c r="F233" t="n">
         <v>0</v>
@@ -19119,7 +19119,7 @@
         <v>77.76221790001728</v>
       </c>
       <c r="E234" t="n">
-        <v>0</v>
+        <v>4658449</v>
       </c>
       <c r="F234" t="n">
         <v>0.2857142857142857</v>
@@ -19199,7 +19199,7 @@
         <v>71.94467850006185</v>
       </c>
       <c r="E235" t="n">
-        <v>0</v>
+        <v>4563824</v>
       </c>
       <c r="F235" t="n">
         <v>1</v>
@@ -19279,7 +19279,7 @@
         <v>72.01234920008574</v>
       </c>
       <c r="E236" t="n">
-        <v>0</v>
+        <v>4568919</v>
       </c>
       <c r="F236" t="n">
         <v>0</v>
@@ -19359,7 +19359,7 @@
         <v>58.48588820011355</v>
       </c>
       <c r="E237" t="n">
-        <v>0</v>
+        <v>4554958</v>
       </c>
       <c r="F237" t="n">
         <v>0.6666666666666666</v>
@@ -19439,7 +19439,7 @@
         <v>102.7988844000502</v>
       </c>
       <c r="E238" t="n">
-        <v>0</v>
+        <v>4558084</v>
       </c>
       <c r="F238" t="n">
         <v>1</v>
@@ -19519,7 +19519,7 @@
         <v>49.32462189998478</v>
       </c>
       <c r="E239" t="n">
-        <v>0</v>
+        <v>4570137</v>
       </c>
       <c r="F239" t="n">
         <v>1</v>
@@ -19599,7 +19599,7 @@
         <v>47.70011960004922</v>
       </c>
       <c r="E240" t="n">
-        <v>0</v>
+        <v>4555954</v>
       </c>
       <c r="F240" t="n">
         <v>1</v>
@@ -19679,7 +19679,7 @@
         <v>58.45446850010194</v>
       </c>
       <c r="E241" t="n">
-        <v>0</v>
+        <v>4571227</v>
       </c>
       <c r="F241" t="n">
         <v>0.5</v>
@@ -19759,7 +19759,7 @@
         <v>45.84415010001976</v>
       </c>
       <c r="E242" t="n">
-        <v>0</v>
+        <v>4561700</v>
       </c>
       <c r="F242" t="n">
         <v>0.5</v>
@@ -19839,7 +19839,7 @@
         <v>50.75901959999464</v>
       </c>
       <c r="E243" t="n">
-        <v>0</v>
+        <v>4566964</v>
       </c>
       <c r="F243" t="n">
         <v>0</v>
@@ -19919,7 +19919,7 @@
         <v>49.78275040001608</v>
       </c>
       <c r="E244" t="n">
-        <v>0</v>
+        <v>4571872</v>
       </c>
       <c r="F244" t="n">
         <v>0</v>
@@ -19999,7 +19999,7 @@
         <v>49.99801999994088</v>
       </c>
       <c r="E245" t="n">
-        <v>0</v>
+        <v>4558488</v>
       </c>
       <c r="F245" t="n">
         <v>1</v>
@@ -20079,7 +20079,7 @@
         <v>49.93376419995911</v>
       </c>
       <c r="E246" t="n">
-        <v>0</v>
+        <v>4568350</v>
       </c>
       <c r="F246" t="n">
         <v>0.5</v>
@@ -20159,7 +20159,7 @@
         <v>55.40537629998289</v>
       </c>
       <c r="E247" t="n">
-        <v>0</v>
+        <v>4561488</v>
       </c>
       <c r="F247" t="n">
         <v>0</v>
@@ -20239,7 +20239,7 @@
         <v>116.9106796999695</v>
       </c>
       <c r="E248" t="n">
-        <v>0</v>
+        <v>9187092</v>
       </c>
       <c r="F248" t="n">
         <v>0.6666666666666666</v>
@@ -20319,7 +20319,7 @@
         <v>50.85302300006151</v>
       </c>
       <c r="E249" t="n">
-        <v>0</v>
+        <v>4559746</v>
       </c>
       <c r="F249" t="n">
         <v>1</v>
@@ -20399,7 +20399,7 @@
         <v>56.33874240005389</v>
       </c>
       <c r="E250" t="n">
-        <v>0</v>
+        <v>4588821</v>
       </c>
       <c r="F250" t="n">
         <v>0</v>
@@ -20479,7 +20479,7 @@
         <v>61.77177460002713</v>
       </c>
       <c r="E251" t="n">
-        <v>0</v>
+        <v>4611381</v>
       </c>
       <c r="F251" t="n">
         <v>0</v>
@@ -20559,7 +20559,7 @@
         <v>96.01418540009763</v>
       </c>
       <c r="E252" t="n">
-        <v>0</v>
+        <v>4561822</v>
       </c>
       <c r="F252" t="n">
         <v>1</v>
@@ -20639,7 +20639,7 @@
         <v>73.82941730006132</v>
       </c>
       <c r="E253" t="n">
-        <v>0</v>
+        <v>4563006</v>
       </c>
       <c r="F253" t="n">
         <v>0</v>
@@ -20719,7 +20719,7 @@
         <v>47.00780690007377</v>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>4556922</v>
       </c>
       <c r="F254" t="n">
         <v>0</v>
@@ -20799,7 +20799,7 @@
         <v>50.60992519999854</v>
       </c>
       <c r="E255" t="n">
-        <v>0</v>
+        <v>4565742</v>
       </c>
       <c r="F255" t="n">
         <v>1</v>
@@ -20879,7 +20879,7 @@
         <v>55.18194119993132</v>
       </c>
       <c r="E256" t="n">
-        <v>0</v>
+        <v>4586091</v>
       </c>
       <c r="F256" t="n">
         <v>1</v>
@@ -20959,7 +20959,7 @@
         <v>62.06381960003637</v>
       </c>
       <c r="E257" t="n">
-        <v>0</v>
+        <v>4575942</v>
       </c>
       <c r="F257" t="n">
         <v>1</v>
@@ -21039,7 +21039,7 @@
         <v>62.37813849991653</v>
       </c>
       <c r="E258" t="n">
-        <v>0</v>
+        <v>4601110</v>
       </c>
       <c r="F258" t="n">
         <v>1</v>
@@ -21119,7 +21119,7 @@
         <v>93.58968430000823</v>
       </c>
       <c r="E259" t="n">
-        <v>0</v>
+        <v>4594487</v>
       </c>
       <c r="F259" t="n">
         <v>1</v>
@@ -21199,7 +21199,7 @@
         <v>56.89078020001762</v>
       </c>
       <c r="E260" t="n">
-        <v>0</v>
+        <v>4627605</v>
       </c>
       <c r="F260" t="n">
         <v>1</v>
@@ -21279,7 +21279,7 @@
         <v>59.77822890004609</v>
       </c>
       <c r="E261" t="n">
-        <v>0</v>
+        <v>4583313</v>
       </c>
       <c r="F261" t="n">
         <v>1</v>
@@ -21359,7 +21359,7 @@
         <v>61.461737500038</v>
       </c>
       <c r="E262" t="n">
-        <v>0</v>
+        <v>9175247</v>
       </c>
       <c r="F262" t="n">
         <v>1</v>
@@ -21439,7 +21439,7 @@
         <v>58.49928630003706</v>
       </c>
       <c r="E263" t="n">
-        <v>0</v>
+        <v>4570991</v>
       </c>
       <c r="F263" t="n">
         <v>0.25</v>
@@ -21519,7 +21519,7 @@
         <v>56.87937780003995</v>
       </c>
       <c r="E264" t="n">
-        <v>0</v>
+        <v>4579799</v>
       </c>
       <c r="F264" t="n">
         <v>0.6666666666666666</v>
@@ -21599,7 +21599,7 @@
         <v>73.74093939992599</v>
       </c>
       <c r="E265" t="n">
-        <v>0</v>
+        <v>4585046</v>
       </c>
       <c r="F265" t="n">
         <v>1</v>
@@ -21679,7 +21679,7 @@
         <v>60.38235129998066</v>
       </c>
       <c r="E266" t="n">
-        <v>0</v>
+        <v>4556224</v>
       </c>
       <c r="F266" t="n">
         <v>0.5</v>
@@ -21759,7 +21759,7 @@
         <v>49.06152099999599</v>
       </c>
       <c r="E267" t="n">
-        <v>0</v>
+        <v>4568486</v>
       </c>
       <c r="F267" t="n">
         <v>0.5</v>
@@ -21839,7 +21839,7 @@
         <v>56.89967770001385</v>
       </c>
       <c r="E268" t="n">
-        <v>0</v>
+        <v>4595711</v>
       </c>
       <c r="F268" t="n">
         <v>1</v>
@@ -21919,7 +21919,7 @@
         <v>87.98951889993623</v>
       </c>
       <c r="E269" t="n">
-        <v>0</v>
+        <v>4601774</v>
       </c>
       <c r="F269" t="n">
         <v>0.5</v>
@@ -21999,7 +21999,7 @@
         <v>60.94568599993363</v>
       </c>
       <c r="E270" t="n">
-        <v>0</v>
+        <v>4600079</v>
       </c>
       <c r="F270" t="n">
         <v>0.4</v>
@@ -22079,7 +22079,7 @@
         <v>60.73527419997845</v>
       </c>
       <c r="E271" t="n">
-        <v>0</v>
+        <v>4596008</v>
       </c>
       <c r="F271" t="n">
         <v>1</v>
@@ -22159,7 +22159,7 @@
         <v>54.23792260000482</v>
       </c>
       <c r="E272" t="n">
-        <v>0</v>
+        <v>4591033</v>
       </c>
       <c r="F272" t="n">
         <v>0.8333333333333334</v>
@@ -22239,7 +22239,7 @@
         <v>57.83596029994078</v>
       </c>
       <c r="E273" t="n">
-        <v>0</v>
+        <v>4614374</v>
       </c>
       <c r="F273" t="n">
         <v>0.6</v>
@@ -22319,7 +22319,7 @@
         <v>50.11489920003805</v>
       </c>
       <c r="E274" t="n">
-        <v>0</v>
+        <v>4573018</v>
       </c>
       <c r="F274" t="n">
         <v>0.75</v>
@@ -22399,7 +22399,7 @@
         <v>56.32400970009621</v>
       </c>
       <c r="E275" t="n">
-        <v>0</v>
+        <v>4589884</v>
       </c>
       <c r="F275" t="n">
         <v>1</v>
@@ -22479,7 +22479,7 @@
         <v>106.1872694999911</v>
       </c>
       <c r="E276" t="n">
-        <v>0</v>
+        <v>9122187</v>
       </c>
       <c r="F276" t="n">
         <v>0.4285714285714285</v>
@@ -22559,7 +22559,7 @@
         <v>54.02301340003032</v>
       </c>
       <c r="E277" t="n">
-        <v>0</v>
+        <v>9117079</v>
       </c>
       <c r="F277" t="n">
         <v>0.5555555555555556</v>
@@ -22639,7 +22639,7 @@
         <v>47.91878119995818</v>
       </c>
       <c r="E278" t="n">
-        <v>0</v>
+        <v>9126403</v>
       </c>
       <c r="F278" t="n">
         <v>1</v>
@@ -22719,7 +22719,7 @@
         <v>56.92887259996496</v>
       </c>
       <c r="E279" t="n">
-        <v>0</v>
+        <v>9633266</v>
       </c>
       <c r="F279" t="n">
         <v>0.6666666666666666</v>
@@ -22799,7 +22799,7 @@
         <v>73.44265629991423</v>
       </c>
       <c r="E280" t="n">
-        <v>0</v>
+        <v>4593722</v>
       </c>
       <c r="F280" t="n">
         <v>0</v>
@@ -22879,7 +22879,7 @@
         <v>50.49898100004066</v>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>4557418</v>
       </c>
       <c r="F281" t="n">
         <v>0.6</v>
@@ -22959,7 +22959,7 @@
         <v>92.67319899995346</v>
       </c>
       <c r="E282" t="n">
-        <v>0</v>
+        <v>4551896</v>
       </c>
       <c r="F282" t="n">
         <v>0.6666666666666666</v>
@@ -23039,7 +23039,7 @@
         <v>44.53680350002833</v>
       </c>
       <c r="E283" t="n">
-        <v>0</v>
+        <v>4565393</v>
       </c>
       <c r="F283" t="n">
         <v>0</v>
@@ -23119,7 +23119,7 @@
         <v>62.72354080004152</v>
       </c>
       <c r="E284" t="n">
-        <v>0</v>
+        <v>4575513</v>
       </c>
       <c r="F284" t="n">
         <v>0.75</v>
@@ -23199,7 +23199,7 @@
         <v>53.25058679992799</v>
       </c>
       <c r="E285" t="n">
-        <v>0</v>
+        <v>4572481</v>
       </c>
       <c r="F285" t="n">
         <v>1</v>
@@ -23279,7 +23279,7 @@
         <v>45.38502809999045</v>
       </c>
       <c r="E286" t="n">
-        <v>0</v>
+        <v>4567036</v>
       </c>
       <c r="F286" t="n">
         <v>0.6666666666666666</v>
@@ -23359,7 +23359,7 @@
         <v>46.55752839997876</v>
       </c>
       <c r="E287" t="n">
-        <v>0</v>
+        <v>4569719</v>
       </c>
       <c r="F287" t="n">
         <v>0.3</v>
@@ -23439,7 +23439,7 @@
         <v>50.93227130000014</v>
       </c>
       <c r="E288" t="n">
-        <v>0</v>
+        <v>4584229</v>
       </c>
       <c r="F288" t="n">
         <v>0.4615384615384616</v>
@@ -23519,7 +23519,7 @@
         <v>45.76925150002353</v>
       </c>
       <c r="E289" t="n">
-        <v>0</v>
+        <v>4558110</v>
       </c>
       <c r="F289" t="n">
         <v>0.75</v>
@@ -23599,7 +23599,7 @@
         <v>45.43896850000601</v>
       </c>
       <c r="E290" t="n">
-        <v>0</v>
+        <v>4568011</v>
       </c>
       <c r="F290" t="n">
         <v>0.6666666666666666</v>
@@ -23679,7 +23679,7 @@
         <v>44.69218670006376</v>
       </c>
       <c r="E291" t="n">
-        <v>0</v>
+        <v>4573912</v>
       </c>
       <c r="F291" t="n">
         <v>0.75</v>
@@ -23759,7 +23759,7 @@
         <v>99.7311425000662</v>
       </c>
       <c r="E292" t="n">
-        <v>0</v>
+        <v>4617430</v>
       </c>
       <c r="F292" t="n">
         <v>0.75</v>
@@ -23839,7 +23839,7 @@
         <v>103.7974405999994</v>
       </c>
       <c r="E293" t="n">
-        <v>0</v>
+        <v>4585683</v>
       </c>
       <c r="F293" t="n">
         <v>1</v>
@@ -23919,7 +23919,7 @@
         <v>102.9408037000103</v>
       </c>
       <c r="E294" t="n">
-        <v>0</v>
+        <v>4591365</v>
       </c>
       <c r="F294" t="n">
         <v>0.6428571428571429</v>
@@ -23999,7 +23999,7 @@
         <v>111.2769088000059</v>
       </c>
       <c r="E295" t="n">
-        <v>0</v>
+        <v>4588194</v>
       </c>
       <c r="F295" t="n">
         <v>0.6923076923076923</v>
@@ -24079,7 +24079,7 @@
         <v>99.13282850000542</v>
       </c>
       <c r="E296" t="n">
-        <v>0</v>
+        <v>4554778</v>
       </c>
       <c r="F296" t="n">
         <v>1</v>
@@ -24159,7 +24159,7 @@
         <v>95.35141100001056</v>
       </c>
       <c r="E297" t="n">
-        <v>0</v>
+        <v>4558103</v>
       </c>
       <c r="F297" t="n">
         <v>0.5</v>
@@ -24239,7 +24239,7 @@
         <v>103.9857347999932</v>
       </c>
       <c r="E298" t="n">
-        <v>0</v>
+        <v>4575804</v>
       </c>
       <c r="F298" t="n">
         <v>0.375</v>
@@ -24319,7 +24319,7 @@
         <v>105.7252485998906</v>
       </c>
       <c r="E299" t="n">
-        <v>0</v>
+        <v>4586653</v>
       </c>
       <c r="F299" t="n">
         <v>0.9166666666666666</v>
@@ -24399,7 +24399,7 @@
         <v>107.4000434000045</v>
       </c>
       <c r="E300" t="n">
-        <v>0</v>
+        <v>4584598</v>
       </c>
       <c r="F300" t="n">
         <v>0.375</v>
@@ -24479,7 +24479,7 @@
         <v>103.1541223999811</v>
       </c>
       <c r="E301" t="n">
-        <v>0</v>
+        <v>4595354</v>
       </c>
       <c r="F301" t="n">
         <v>0.75</v>
@@ -24559,7 +24559,7 @@
         <v>142.5418609000044</v>
       </c>
       <c r="E302" t="n">
-        <v>0</v>
+        <v>1676444</v>
       </c>
       <c r="F302" t="n">
         <v>1</v>
@@ -24639,7 +24639,7 @@
         <v>51.99675200006459</v>
       </c>
       <c r="E303" t="n">
-        <v>0</v>
+        <v>1672378</v>
       </c>
       <c r="F303" t="n">
         <v>0.8333333333333334</v>
@@ -24719,7 +24719,7 @@
         <v>50.06366059998982</v>
       </c>
       <c r="E304" t="n">
-        <v>0</v>
+        <v>1667988</v>
       </c>
       <c r="F304" t="n">
         <v>1</v>
@@ -24799,7 +24799,7 @@
         <v>52.06516290002037</v>
       </c>
       <c r="E305" t="n">
-        <v>0</v>
+        <v>1672642</v>
       </c>
       <c r="F305" t="n">
         <v>1</v>
@@ -24879,7 +24879,7 @@
         <v>53.49238399998285</v>
       </c>
       <c r="E306" t="n">
-        <v>0</v>
+        <v>1678909</v>
       </c>
       <c r="F306" t="n">
         <v>0.8571428571428571</v>
@@ -24959,7 +24959,7 @@
         <v>49.33268270001281</v>
       </c>
       <c r="E307" t="n">
-        <v>0</v>
+        <v>1670387</v>
       </c>
       <c r="F307" t="n">
         <v>0.7857142857142857</v>
@@ -25039,7 +25039,7 @@
         <v>51.21489249996375</v>
       </c>
       <c r="E308" t="n">
-        <v>0</v>
+        <v>1670640</v>
       </c>
       <c r="F308" t="n">
         <v>1</v>
@@ -25119,7 +25119,7 @@
         <v>60.37563579995185</v>
       </c>
       <c r="E309" t="n">
-        <v>0</v>
+        <v>1683538</v>
       </c>
       <c r="F309" t="n">
         <v>1</v>
@@ -25199,7 +25199,7 @@
         <v>49.0841478999937</v>
       </c>
       <c r="E310" t="n">
-        <v>0</v>
+        <v>1666389</v>
       </c>
       <c r="F310" t="n">
         <v>0.7142857142857143</v>
@@ -25279,7 +25279,7 @@
         <v>55.74774609995075</v>
       </c>
       <c r="E311" t="n">
-        <v>0</v>
+        <v>1668217</v>
       </c>
       <c r="F311" t="n">
         <v>0.8</v>
@@ -25359,7 +25359,7 @@
         <v>51.72289779991843</v>
       </c>
       <c r="E312" t="n">
-        <v>0</v>
+        <v>1669023</v>
       </c>
       <c r="F312" t="n">
         <v>0.8333333333333334</v>
@@ -25439,7 +25439,7 @@
         <v>54.10562679998111</v>
       </c>
       <c r="E313" t="n">
-        <v>0</v>
+        <v>1670533</v>
       </c>
       <c r="F313" t="n">
         <v>0.625</v>
@@ -25519,7 +25519,7 @@
         <v>57.89882660005242</v>
       </c>
       <c r="E314" t="n">
-        <v>0</v>
+        <v>1668569</v>
       </c>
       <c r="F314" t="n">
         <v>0.6666666666666666</v>
@@ -25599,7 +25599,7 @@
         <v>50.15031310007907</v>
       </c>
       <c r="E315" t="n">
-        <v>0</v>
+        <v>1671439</v>
       </c>
       <c r="F315" t="n">
         <v>1</v>
@@ -25679,7 +25679,7 @@
         <v>52.67111780005507</v>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>1665428</v>
       </c>
       <c r="F316" t="n">
         <v>0.4285714285714285</v>
@@ -25759,7 +25759,7 @@
         <v>143.8650142000988</v>
       </c>
       <c r="E317" t="n">
-        <v>0</v>
+        <v>1674310</v>
       </c>
       <c r="F317" t="n">
         <v>0.8571428571428571</v>
@@ -25839,7 +25839,7 @@
         <v>50.67637980007567</v>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>1669232</v>
       </c>
       <c r="F318" t="n">
         <v>0.5</v>
@@ -25919,7 +25919,7 @@
         <v>53.79260829999112</v>
       </c>
       <c r="E319" t="n">
-        <v>0</v>
+        <v>1667841</v>
       </c>
       <c r="F319" t="n">
         <v>1</v>
@@ -25999,7 +25999,7 @@
         <v>61.86383089993615</v>
       </c>
       <c r="E320" t="n">
-        <v>0</v>
+        <v>1683300</v>
       </c>
       <c r="F320" t="n">
         <v>0.6428571428571429</v>
@@ -26079,7 +26079,7 @@
         <v>49.87838369992096</v>
       </c>
       <c r="E321" t="n">
-        <v>0</v>
+        <v>1668956</v>
       </c>
       <c r="F321" t="n">
         <v>0.8571428571428571</v>
@@ -26159,7 +26159,7 @@
         <v>48.57794890005607</v>
       </c>
       <c r="E322" t="n">
-        <v>0</v>
+        <v>1665800</v>
       </c>
       <c r="F322" t="n">
         <v>0.6666666666666666</v>
@@ -26239,7 +26239,7 @@
         <v>48.22828450007364</v>
       </c>
       <c r="E323" t="n">
-        <v>0</v>
+        <v>1663083</v>
       </c>
       <c r="F323" t="n">
         <v>0.5</v>
@@ -26319,7 +26319,7 @@
         <v>49.50069929996971</v>
       </c>
       <c r="E324" t="n">
-        <v>0</v>
+        <v>1667964</v>
       </c>
       <c r="F324" t="n">
         <v>0.5714285714285714</v>
@@ -26399,7 +26399,7 @@
         <v>49.68789689999539</v>
       </c>
       <c r="E325" t="n">
-        <v>0</v>
+        <v>1672177</v>
       </c>
       <c r="F325" t="n">
         <v>0.75</v>
@@ -26479,7 +26479,7 @@
         <v>52.6550525999628</v>
       </c>
       <c r="E326" t="n">
-        <v>0</v>
+        <v>1676318</v>
       </c>
       <c r="F326" t="n">
         <v>0.7272727272727273</v>
@@ -26559,7 +26559,7 @@
         <v>52.87636029999703</v>
       </c>
       <c r="E327" t="n">
-        <v>0</v>
+        <v>1672296</v>
       </c>
       <c r="F327" t="n">
         <v>0.7142857142857143</v>
@@ -26639,7 +26639,7 @@
         <v>37.02152999991085</v>
       </c>
       <c r="E328" t="n">
-        <v>0</v>
+        <v>1680547</v>
       </c>
       <c r="F328" t="n">
         <v>0.6666666666666666</v>
@@ -26719,7 +26719,7 @@
         <v>36.23663870000746</v>
       </c>
       <c r="E329" t="n">
-        <v>0</v>
+        <v>1675751</v>
       </c>
       <c r="F329" t="n">
         <v>0.8888888888888888</v>
@@ -26799,7 +26799,7 @@
         <v>38.08472139993683</v>
       </c>
       <c r="E330" t="n">
-        <v>0</v>
+        <v>1677048</v>
       </c>
       <c r="F330" t="n">
         <v>0.5454545454545454</v>
@@ -26879,7 +26879,7 @@
         <v>32.2362936999416</v>
       </c>
       <c r="E331" t="n">
-        <v>0</v>
+        <v>1671905</v>
       </c>
       <c r="F331" t="n">
         <v>0.6666666666666666</v>
@@ -26959,7 +26959,7 @@
         <v>32.99854790000245</v>
       </c>
       <c r="E332" t="n">
-        <v>0</v>
+        <v>1678657</v>
       </c>
       <c r="F332" t="n">
         <v>0.8888888888888888</v>
@@ -27039,7 +27039,7 @@
         <v>31.27510219998658</v>
       </c>
       <c r="E333" t="n">
-        <v>0</v>
+        <v>1665407</v>
       </c>
       <c r="F333" t="n">
         <v>0.5714285714285714</v>
@@ -27119,7 +27119,7 @@
         <v>57.23341240000445</v>
       </c>
       <c r="E334" t="n">
-        <v>0</v>
+        <v>1680996</v>
       </c>
       <c r="F334" t="n">
         <v>0.6666666666666666</v>
@@ -27199,7 +27199,7 @@
         <v>52.31141890003346</v>
       </c>
       <c r="E335" t="n">
-        <v>0</v>
+        <v>1670160</v>
       </c>
       <c r="F335" t="n">
         <v>1</v>
@@ -27279,7 +27279,7 @@
         <v>52.04424290009774</v>
       </c>
       <c r="E336" t="n">
-        <v>0</v>
+        <v>1669080</v>
       </c>
       <c r="F336" t="n">
         <v>1</v>
@@ -27359,7 +27359,7 @@
         <v>52.55977480008733</v>
       </c>
       <c r="E337" t="n">
-        <v>0</v>
+        <v>1674414</v>
       </c>
       <c r="F337" t="n">
         <v>1</v>
@@ -27439,7 +27439,7 @@
         <v>56.38668620004319</v>
       </c>
       <c r="E338" t="n">
-        <v>0</v>
+        <v>1674200</v>
       </c>
       <c r="F338" t="n">
         <v>0.7</v>
@@ -27519,7 +27519,7 @@
         <v>59.59052570001222</v>
       </c>
       <c r="E339" t="n">
-        <v>0</v>
+        <v>1676526</v>
       </c>
       <c r="F339" t="n">
         <v>0.7272727272727273</v>
@@ -27599,7 +27599,7 @@
         <v>61.68258580006659</v>
       </c>
       <c r="E340" t="n">
-        <v>0</v>
+        <v>1668068</v>
       </c>
       <c r="F340" t="n">
         <v>1</v>
@@ -27679,7 +27679,7 @@
         <v>60.2881651999196</v>
       </c>
       <c r="E341" t="n">
-        <v>0</v>
+        <v>1682431</v>
       </c>
       <c r="F341" t="n">
         <v>0.8333333333333334</v>
@@ -27759,7 +27759,7 @@
         <v>61.63464359997306</v>
       </c>
       <c r="E342" t="n">
-        <v>0</v>
+        <v>1687967</v>
       </c>
       <c r="F342" t="n">
         <v>0.6666666666666666</v>
@@ -27839,7 +27839,7 @@
         <v>54.05210530001204</v>
       </c>
       <c r="E343" t="n">
-        <v>0</v>
+        <v>1680425</v>
       </c>
       <c r="F343" t="n">
         <v>0.625</v>
@@ -27919,7 +27919,7 @@
         <v>56.21710880007595</v>
       </c>
       <c r="E344" t="n">
-        <v>0</v>
+        <v>1686946</v>
       </c>
       <c r="F344" t="n">
         <v>0.75</v>
@@ -27999,7 +27999,7 @@
         <v>58.21852599992417</v>
       </c>
       <c r="E345" t="n">
-        <v>0</v>
+        <v>1689336</v>
       </c>
       <c r="F345" t="n">
         <v>0.6666666666666666</v>
@@ -28079,7 +28079,7 @@
         <v>52.81378660001792</v>
       </c>
       <c r="E346" t="n">
-        <v>0</v>
+        <v>1670232</v>
       </c>
       <c r="F346" t="n">
         <v>1</v>
@@ -28159,7 +28159,7 @@
         <v>33.9233702000929</v>
       </c>
       <c r="E347" t="n">
-        <v>0</v>
+        <v>1667791</v>
       </c>
       <c r="F347" t="n">
         <v>0.5</v>
@@ -28239,7 +28239,7 @@
         <v>30.07409310003277</v>
       </c>
       <c r="E348" t="n">
-        <v>0</v>
+        <v>1673093</v>
       </c>
       <c r="F348" t="n">
         <v>0.7777777777777778</v>
@@ -28319,7 +28319,7 @@
         <v>27.38108280010056</v>
       </c>
       <c r="E349" t="n">
-        <v>0</v>
+        <v>1663001</v>
       </c>
       <c r="F349" t="n">
         <v>1</v>
@@ -28399,7 +28399,7 @@
         <v>33.05646580003668</v>
       </c>
       <c r="E350" t="n">
-        <v>0</v>
+        <v>1669628</v>
       </c>
       <c r="F350" t="n">
         <v>1</v>
@@ -28479,7 +28479,7 @@
         <v>28.7813610000303</v>
       </c>
       <c r="E351" t="n">
-        <v>0</v>
+        <v>1670826</v>
       </c>
       <c r="F351" t="n">
         <v>0.8333333333333334</v>
@@ -28559,7 +28559,7 @@
         <v>27.42527770006564</v>
       </c>
       <c r="E352" t="n">
-        <v>0</v>
+        <v>1671481</v>
       </c>
       <c r="F352" t="n">
         <v>1</v>
@@ -28639,7 +28639,7 @@
         <v>32.17526629997883</v>
       </c>
       <c r="E353" t="n">
-        <v>0</v>
+        <v>1668509</v>
       </c>
       <c r="F353" t="n">
         <v>0.6666666666666666</v>
@@ -28719,7 +28719,7 @@
         <v>39.84968850004952</v>
       </c>
       <c r="E354" t="n">
-        <v>0</v>
+        <v>1668311</v>
       </c>
       <c r="F354" t="n">
         <v>1</v>
@@ -28799,7 +28799,7 @@
         <v>29.61869919998571</v>
       </c>
       <c r="E355" t="n">
-        <v>0</v>
+        <v>1673991</v>
       </c>
       <c r="F355" t="n">
         <v>1</v>
@@ -28879,7 +28879,7 @@
         <v>34.14172650000546</v>
       </c>
       <c r="E356" t="n">
-        <v>0</v>
+        <v>1684228</v>
       </c>
       <c r="F356" t="n">
         <v>0.8333333333333334</v>
@@ -28959,7 +28959,7 @@
         <v>27.46754680003505</v>
       </c>
       <c r="E357" t="n">
-        <v>0</v>
+        <v>1668795</v>
       </c>
       <c r="F357" t="n">
         <v>0.7777777777777778</v>
@@ -29039,7 +29039,7 @@
         <v>33.14618649997283</v>
       </c>
       <c r="E358" t="n">
-        <v>0</v>
+        <v>1669063</v>
       </c>
       <c r="F358" t="n">
         <v>0.8</v>
@@ -29119,7 +29119,7 @@
         <v>28.9374092000071</v>
       </c>
       <c r="E359" t="n">
-        <v>0</v>
+        <v>1665306</v>
       </c>
       <c r="F359" t="n">
         <v>0.6666666666666666</v>
@@ -29199,7 +29199,7 @@
         <v>32.92567079991568</v>
       </c>
       <c r="E360" t="n">
-        <v>0</v>
+        <v>1679423</v>
       </c>
       <c r="F360" t="n">
         <v>0.5454545454545454</v>
@@ -29279,7 +29279,7 @@
         <v>31.13230410008691</v>
       </c>
       <c r="E361" t="n">
-        <v>0</v>
+        <v>1680209</v>
       </c>
       <c r="F361" t="n">
         <v>0.9090909090909091</v>
@@ -29359,7 +29359,7 @@
         <v>31.71762699994724</v>
       </c>
       <c r="E362" t="n">
-        <v>0</v>
+        <v>1662226</v>
       </c>
       <c r="F362" t="n">
         <v>1</v>
@@ -29439,7 +29439,7 @@
         <v>33.40011279995088</v>
       </c>
       <c r="E363" t="n">
-        <v>0</v>
+        <v>1670884</v>
       </c>
       <c r="F363" t="n">
         <v>0.8333333333333334</v>
@@ -29519,7 +29519,7 @@
         <v>32.24232530000154</v>
       </c>
       <c r="E364" t="n">
-        <v>0</v>
+        <v>1675079</v>
       </c>
       <c r="F364" t="n">
         <v>0.7</v>
@@ -29599,7 +29599,7 @@
         <v>22.31740739999805</v>
       </c>
       <c r="E365" t="n">
-        <v>0</v>
+        <v>768709</v>
       </c>
       <c r="F365" t="n">
         <v>1</v>
@@ -29679,7 +29679,7 @@
         <v>19.49598160001915</v>
       </c>
       <c r="E366" t="n">
-        <v>0</v>
+        <v>768656</v>
       </c>
       <c r="F366" t="n">
         <v>1</v>
@@ -29759,7 +29759,7 @@
         <v>19.79638000007253</v>
       </c>
       <c r="E367" t="n">
-        <v>0</v>
+        <v>769521</v>
       </c>
       <c r="F367" t="n">
         <v>1</v>
@@ -29839,7 +29839,7 @@
         <v>24.57817209989298</v>
       </c>
       <c r="E368" t="n">
-        <v>0</v>
+        <v>770691</v>
       </c>
       <c r="F368" t="n">
         <v>1</v>
@@ -29919,7 +29919,7 @@
         <v>29.2064049000619</v>
       </c>
       <c r="E369" t="n">
-        <v>0</v>
+        <v>769269</v>
       </c>
       <c r="F369" t="n">
         <v>1</v>
@@ -29999,7 +29999,7 @@
         <v>19.67860710003879</v>
       </c>
       <c r="E370" t="n">
-        <v>0</v>
+        <v>769206</v>
       </c>
       <c r="F370" t="n">
         <v>1</v>
@@ -30079,7 +30079,7 @@
         <v>21.14798629994038</v>
       </c>
       <c r="E371" t="n">
-        <v>0</v>
+        <v>769707</v>
       </c>
       <c r="F371" t="n">
         <v>1</v>
@@ -30159,7 +30159,7 @@
         <v>40.93163799995091</v>
       </c>
       <c r="E372" t="n">
-        <v>0</v>
+        <v>775157</v>
       </c>
       <c r="F372" t="n">
         <v>1</v>
@@ -30239,7 +30239,7 @@
         <v>41.05044839996845</v>
       </c>
       <c r="E373" t="n">
-        <v>0</v>
+        <v>770260</v>
       </c>
       <c r="F373" t="n">
         <v>0.6</v>
@@ -30319,7 +30319,7 @@
         <v>38.68370509997476</v>
       </c>
       <c r="E374" t="n">
-        <v>0</v>
+        <v>769145</v>
       </c>
       <c r="F374" t="n">
         <v>1</v>
@@ -30399,7 +30399,7 @@
         <v>38.20471089996863</v>
       </c>
       <c r="E375" t="n">
-        <v>0</v>
+        <v>770810</v>
       </c>
       <c r="F375" t="n">
         <v>1</v>
@@ -30479,7 +30479,7 @@
         <v>49.2981940000318</v>
       </c>
       <c r="E376" t="n">
-        <v>0</v>
+        <v>770565</v>
       </c>
       <c r="F376" t="n">
         <v>0.6666666666666666</v>
@@ -30559,7 +30559,7 @@
         <v>39.29012170003261</v>
       </c>
       <c r="E377" t="n">
-        <v>0</v>
+        <v>772782</v>
       </c>
       <c r="F377" t="n">
         <v>0.5714285714285714</v>
@@ -30639,7 +30639,7 @@
         <v>46.76399020000827</v>
       </c>
       <c r="E378" t="n">
-        <v>0</v>
+        <v>773667</v>
       </c>
       <c r="F378" t="n">
         <v>0.8</v>
@@ -30719,7 +30719,7 @@
         <v>38.48300979996566</v>
       </c>
       <c r="E379" t="n">
-        <v>0</v>
+        <v>770113</v>
       </c>
       <c r="F379" t="n">
         <v>1</v>
@@ -30799,7 +30799,7 @@
         <v>44.96213869994972</v>
       </c>
       <c r="E380" t="n">
-        <v>0</v>
+        <v>769189</v>
       </c>
       <c r="F380" t="n">
         <v>1</v>
@@ -30879,7 +30879,7 @@
         <v>38.0036769999424</v>
       </c>
       <c r="E381" t="n">
-        <v>0</v>
+        <v>771052</v>
       </c>
       <c r="F381" t="n">
         <v>0.5555555555555556</v>
@@ -30959,7 +30959,7 @@
         <v>48.17845580005087</v>
       </c>
       <c r="E382" t="n">
-        <v>0</v>
+        <v>771469</v>
       </c>
       <c r="F382" t="n">
         <v>0.7142857142857143</v>
@@ -31039,7 +31039,7 @@
         <v>34.71891699999105</v>
       </c>
       <c r="E383" t="n">
-        <v>0</v>
+        <v>769710</v>
       </c>
       <c r="F383" t="n">
         <v>1</v>
@@ -31119,7 +31119,7 @@
         <v>30.52466179989278</v>
       </c>
       <c r="E384" t="n">
-        <v>0</v>
+        <v>772805</v>
       </c>
       <c r="F384" t="n">
         <v>0.4285714285714285</v>
@@ -31199,7 +31199,7 @@
         <v>30.48415410006419</v>
       </c>
       <c r="E385" t="n">
-        <v>0</v>
+        <v>769056</v>
       </c>
       <c r="F385" t="n">
         <v>0.6</v>
@@ -31279,7 +31279,7 @@
         <v>24.18192950007506</v>
       </c>
       <c r="E386" t="n">
-        <v>0</v>
+        <v>769853</v>
       </c>
       <c r="F386" t="n">
         <v>0.6666666666666666</v>
@@ -31359,7 +31359,7 @@
         <v>23.4485709000146</v>
       </c>
       <c r="E387" t="n">
-        <v>0</v>
+        <v>769824</v>
       </c>
       <c r="F387" t="n">
         <v>1</v>
@@ -31439,7 +31439,7 @@
         <v>23.20955210004468</v>
       </c>
       <c r="E388" t="n">
-        <v>0</v>
+        <v>772257</v>
       </c>
       <c r="F388" t="n">
         <v>1</v>
@@ -31519,7 +31519,7 @@
         <v>27.68215030001011</v>
       </c>
       <c r="E389" t="n">
-        <v>0</v>
+        <v>774313</v>
       </c>
       <c r="F389" t="n">
         <v>1</v>
@@ -31599,7 +31599,7 @@
         <v>25.79129540000577</v>
       </c>
       <c r="E390" t="n">
-        <v>0</v>
+        <v>771040</v>
       </c>
       <c r="F390" t="n">
         <v>0.6</v>
@@ -31679,7 +31679,7 @@
         <v>29.2312707999954</v>
       </c>
       <c r="E391" t="n">
-        <v>0</v>
+        <v>769774</v>
       </c>
       <c r="F391" t="n">
         <v>1</v>
@@ -31759,7 +31759,7 @@
         <v>22.42029080004431</v>
       </c>
       <c r="E392" t="n">
-        <v>0</v>
+        <v>769576</v>
       </c>
       <c r="F392" t="n">
         <v>0.5</v>
@@ -31839,7 +31839,7 @@
         <v>28.90721440000925</v>
       </c>
       <c r="E393" t="n">
-        <v>0</v>
+        <v>770863</v>
       </c>
       <c r="F393" t="n">
         <v>0.625</v>
@@ -31919,7 +31919,7 @@
         <v>32.48111640010029</v>
       </c>
       <c r="E394" t="n">
-        <v>0</v>
+        <v>773978</v>
       </c>
       <c r="F394" t="n">
         <v>0.5833333333333334</v>
@@ -31999,7 +31999,7 @@
         <v>26.55737200006843</v>
       </c>
       <c r="E395" t="n">
-        <v>0</v>
+        <v>772618</v>
       </c>
       <c r="F395" t="n">
         <v>0.5714285714285714</v>
@@ -32079,7 +32079,7 @@
         <v>27.19612800003961</v>
       </c>
       <c r="E396" t="n">
-        <v>0</v>
+        <v>774245</v>
       </c>
       <c r="F396" t="n">
         <v>0.75</v>
@@ -32159,7 +32159,7 @@
         <v>28.9117662999779</v>
       </c>
       <c r="E397" t="n">
-        <v>0</v>
+        <v>773593</v>
       </c>
       <c r="F397" t="n">
         <v>1</v>
@@ -32239,7 +32239,7 @@
         <v>23.72389210003894</v>
       </c>
       <c r="E398" t="n">
-        <v>0</v>
+        <v>770450</v>
       </c>
       <c r="F398" t="n">
         <v>0.75</v>
@@ -32319,7 +32319,7 @@
         <v>20.98771860008128</v>
       </c>
       <c r="E399" t="n">
-        <v>0</v>
+        <v>771207</v>
       </c>
       <c r="F399" t="n">
         <v>0.5454545454545454</v>
@@ -32399,7 +32399,7 @@
         <v>27.28880109998863</v>
       </c>
       <c r="E400" t="n">
-        <v>0</v>
+        <v>772441</v>
       </c>
       <c r="F400" t="n">
         <v>0.4545454545454545</v>
@@ -32479,7 +32479,7 @@
         <v>26.4384635000024</v>
       </c>
       <c r="E401" t="n">
-        <v>0</v>
+        <v>773089</v>
       </c>
       <c r="F401" t="n">
         <v>0.5714285714285714</v>
@@ -32559,7 +32559,7 @@
         <v>22.90152880002279</v>
       </c>
       <c r="E402" t="n">
-        <v>0</v>
+        <v>773721</v>
       </c>
       <c r="F402" t="n">
         <v>0.6666666666666666</v>
@@ -32639,7 +32639,7 @@
         <v>31.02441459998954</v>
       </c>
       <c r="E403" t="n">
-        <v>0</v>
+        <v>782560</v>
       </c>
       <c r="F403" t="n">
         <v>0.9487179487179487</v>
@@ -32719,7 +32719,7 @@
         <v>26.91103700001258</v>
       </c>
       <c r="E404" t="n">
-        <v>0</v>
+        <v>771036</v>
       </c>
       <c r="F404" t="n">
         <v>0.4347826086956522</v>

</xml_diff>